<commit_message>
Added pin assigment to scheme
</commit_message>
<xml_diff>
--- a/drive_bld300b_interface_board/DOCS/PinAssignment.xlsx
+++ b/drive_bld300b_interface_board/DOCS/PinAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\francor\francor_electronics\drive_bld300b_interface_board\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9648D7C2-E87B-4B86-93DC-C80ACA60DFB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD695C5-A05E-4229-ADA0-0565756BA217}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{C7EC259D-A9A8-437A-8C6E-42677D8F9300}"/>
   </bookViews>
@@ -310,11 +310,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -632,52 +632,52 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K4" sqref="K4:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -685,25 +685,25 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>57</v>
       </c>
       <c r="J3" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -711,25 +711,25 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>58</v>
       </c>
       <c r="J4" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -737,25 +737,25 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>56</v>
       </c>
       <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="J5" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -763,25 +763,25 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>60</v>
       </c>
       <c r="J6" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -789,25 +789,25 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>76</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>75</v>
       </c>
       <c r="G7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J7" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -815,25 +815,25 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G8" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="J8" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -841,25 +841,25 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G9" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>62</v>
       </c>
       <c r="J9" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="2" t="s">
         <v>70</v>
       </c>
     </row>
@@ -867,25 +867,25 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G10" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>63</v>
       </c>
       <c r="J10" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -893,25 +893,25 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G11" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>64</v>
       </c>
       <c r="J11" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="2" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added scheme and PCB
</commit_message>
<xml_diff>
--- a/drive_bld300b_interface_board/DOCS/PinAssignment.xlsx
+++ b/drive_bld300b_interface_board/DOCS/PinAssignment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\francor\francor_electronics\drive_bld300b_interface_board\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD695C5-A05E-4229-ADA0-0565756BA217}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A0093D-3456-4D69-AC58-D2884509889D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{C7EC259D-A9A8-437A-8C6E-42677D8F9300}"/>
+    <workbookView xWindow="15930" yWindow="8280" windowWidth="28800" windowHeight="15435" xr2:uid="{C7EC259D-A9A8-437A-8C6E-42677D8F9300}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K11"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>